<commit_message>
code cleanup and change hardware design
In the powerup process, the mic output waveform will rise up to 1.5 dc voltage in 1sec due to input high pass filter. To improve the speed, I change the capacitor from 1uf to 100nf, result in 400ms rise up time.
</commit_message>
<xml_diff>
--- a/hardware/PCB/BOM.xlsx
+++ b/hardware/PCB/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="18468" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="电子元件" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="212">
   <si>
     <t>Item</t>
   </si>
@@ -203,7 +203,7 @@
     <t>C22</t>
   </si>
   <si>
-    <t>C4,C5,C6,C7,C12,C13,C14,C15,C16,C19,C23,C25</t>
+    <t>C4,C5,C6,C7,C12,C13,C14,C15,C16,C19,C23,C25,C17</t>
   </si>
   <si>
     <t>12</t>
@@ -237,21 +237,6 @@
   </si>
   <si>
     <t>C25808</t>
-  </si>
-  <si>
-    <t>1uF ±10% 50V</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>CL10A105KB8NNNC</t>
-  </si>
-  <si>
-    <t>C15849</t>
   </si>
   <si>
     <t>厚膜电阻 10kΩ ±1% 100mW</t>
@@ -1879,10 +1864,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2296,16 +2281,16 @@
         <v>13</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>18</v>
@@ -2315,29 +2300,29 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="2" t="s">
-        <v>79</v>
+      <c r="A15" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="G15" s="8" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>18</v>
@@ -2347,26 +2332,26 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="17" t="s">
-        <v>85</v>
+      <c r="A16" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>90</v>
@@ -2379,7 +2364,7 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -2388,7 +2373,7 @@
       <c r="C17" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="8" t="s">
@@ -2403,72 +2388,72 @@
       <c r="H17" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>13</v>
-      </c>
+      <c r="D18" s="16"/>
       <c r="E18" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>19</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="15"/>
+      <c r="A19" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="B19" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="16"/>
+        <v>99</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="E19" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+        <v>101</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="2" t="s">
-        <v>103</v>
+      <c r="A20" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>103</v>
@@ -2477,7 +2462,7 @@
         <v>104</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>30</v>
@@ -2486,10 +2471,10 @@
         <v>103</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I20" s="19" t="s">
         <v>18</v>
@@ -2499,29 +2484,29 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="17" t="s">
-        <v>107</v>
+      <c r="A21" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>18</v>
@@ -2532,22 +2517,22 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>116</v>
+        <v>13</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>117</v>
@@ -2573,7 +2558,7 @@
         <v>121</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>30</v>
@@ -2605,19 +2590,19 @@
         <v>126</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I24" s="19" t="s">
         <v>18</v>
@@ -2628,28 +2613,28 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I25" s="19" t="s">
         <v>18</v>
@@ -2660,28 +2645,28 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I26" s="19" t="s">
         <v>18</v>
@@ -2692,25 +2677,25 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>146</v>
+        <v>14</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>147</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>148</v>
@@ -2727,28 +2712,28 @@
         <v>149</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="E28" s="8" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F28" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>153</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>18</v>
+        <v>154</v>
       </c>
       <c r="J28" s="19" t="s">
         <v>19</v>
@@ -2756,31 +2741,31 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>159</v>
+        <v>18</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>19</v>
@@ -2788,28 +2773,28 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I30" s="19" t="s">
         <v>18</v>
@@ -2820,28 +2805,28 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>169</v>
+        <v>13</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I31" s="19" t="s">
         <v>18</v>
@@ -2852,28 +2837,28 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>175</v>
-      </c>
       <c r="G32" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I32" s="19" t="s">
         <v>18</v>
@@ -2884,28 +2869,28 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>181</v>
+        <v>13</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>179</v>
+        <v>15</v>
       </c>
       <c r="G33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="I33" s="19" t="s">
         <v>18</v>
@@ -2915,29 +2900,29 @@
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>15</v>
+        <v>184</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>16</v>
+        <v>187</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I34" s="19" t="s">
         <v>18</v>
@@ -2947,26 +2932,26 @@
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="17" t="s">
-        <v>188</v>
+      <c r="A35" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>191</v>
+        <v>13</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>192</v>
+        <v>16</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>193</v>
@@ -2975,51 +2960,19 @@
         <v>18</v>
       </c>
       <c r="J35" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J36" s="19" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I17:I18"/>
     <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="J17:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3054,10 +3007,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C2" s="4">
         <v>2</v>
@@ -3065,10 +3018,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -3076,10 +3029,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C4" s="6">
         <v>4</v>
@@ -3087,10 +3040,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -3098,10 +3051,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C6" s="6">
         <v>4</v>
@@ -3109,10 +3062,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C7" s="6">
         <v>4</v>
@@ -3120,7 +3073,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6">
@@ -3129,7 +3082,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6">
@@ -3138,10 +3091,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -3149,7 +3102,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="6">
@@ -3158,7 +3111,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7">

</xml_diff>